<commit_message>
only show task when reaction is yes
</commit_message>
<xml_diff>
--- a/cht_app/forms/app/padr.xlsx
+++ b/cht_app/forms/app/padr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="501">
   <si>
     <t>type</t>
   </si>
@@ -310,7 +310,7 @@
     <t>County</t>
   </si>
   <si>
-    <t>minimal</t>
+    <t>autocomplete</t>
   </si>
   <si>
     <t>select_one type</t>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>stop_date_multiple</t>
+  </si>
+  <si>
+    <t>. &lt;= today() and (${start_date_multiple} = '' or . &gt;= ${start_date_multiple})</t>
   </si>
   <si>
     <t>expiry_date_multiple</t>
@@ -6458,11 +6461,11 @@
         <v>158</v>
       </c>
       <c r="L79" s="22"/>
-      <c r="M79" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N79" s="35" t="s">
-        <v>124</v>
+      <c r="M79" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="N79" s="44" t="s">
+        <v>149</v>
       </c>
       <c r="O79" s="27"/>
       <c r="P79" s="27"/>
@@ -6518,11 +6521,11 @@
         <v>158</v>
       </c>
       <c r="L80" s="22"/>
-      <c r="M80" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N80" s="35" t="s">
-        <v>124</v>
+      <c r="M80" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="N80" s="44" t="s">
+        <v>153</v>
       </c>
       <c r="O80" s="27"/>
       <c r="P80" s="27"/>
@@ -6560,7 +6563,7 @@
         <v>120</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>155</v>
@@ -6615,7 +6618,7 @@
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="40" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B82" s="40" t="s">
         <v>162</v>
@@ -6814,10 +6817,10 @@
         <v>34</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D86" s="27"/>
       <c r="E86" s="27"/>
@@ -6866,7 +6869,7 @@
         <v>34</v>
       </c>
       <c r="B87" s="20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C87" s="21" t="s">
         <v>36</v>
@@ -6917,13 +6920,13 @@
     </row>
     <row r="88" ht="18.75" customHeight="1">
       <c r="A88" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D88" s="27"/>
       <c r="E88" s="27"/>
@@ -6974,10 +6977,10 @@
         <v>125</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C89" s="45" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D89" s="27"/>
       <c r="E89" s="27"/>
@@ -7026,10 +7029,10 @@
         <v>134</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D90" s="27"/>
       <c r="E90" s="27"/>
@@ -7041,7 +7044,7 @@
         <v>86</v>
       </c>
       <c r="K90" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L90" s="22"/>
       <c r="M90" s="29" t="s">
@@ -7083,13 +7086,13 @@
     </row>
     <row r="91" ht="18.75" customHeight="1">
       <c r="A91" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C91" s="45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D91" s="27"/>
       <c r="E91" s="27"/>
@@ -7101,7 +7104,7 @@
         <v>86</v>
       </c>
       <c r="K91" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L91" s="36"/>
       <c r="M91" s="27"/>
@@ -7142,10 +7145,10 @@
         <v>83</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D92" s="27"/>
       <c r="E92" s="27"/>
@@ -7155,7 +7158,7 @@
       <c r="I92" s="27"/>
       <c r="J92" s="27"/>
       <c r="K92" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L92" s="22"/>
       <c r="M92" s="27"/>
@@ -7196,10 +7199,10 @@
         <v>131</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D93" s="27"/>
       <c r="E93" s="27"/>
@@ -7209,7 +7212,7 @@
       <c r="I93" s="27"/>
       <c r="J93" s="27"/>
       <c r="K93" s="29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L93" s="22"/>
       <c r="M93" s="27"/>
@@ -7250,7 +7253,7 @@
         <v>161</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C94" s="22" t="s">
         <v>36</v>
@@ -7263,7 +7266,7 @@
       <c r="I94" s="27"/>
       <c r="J94" s="27"/>
       <c r="K94" s="29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L94" s="22"/>
       <c r="M94" s="27"/>
@@ -7287,7 +7290,7 @@
       <c r="AE94" s="27"/>
       <c r="AF94" s="22"/>
       <c r="AG94" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AH94" s="22"/>
       <c r="AI94" s="22"/>
@@ -7303,13 +7306,13 @@
     </row>
     <row r="95" ht="18.75" customHeight="1">
       <c r="A95" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D95" s="27"/>
       <c r="E95" s="27"/>
@@ -7321,7 +7324,7 @@
         <v>86</v>
       </c>
       <c r="K95" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L95" s="36"/>
       <c r="M95" s="27"/>
@@ -7362,10 +7365,10 @@
         <v>83</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D96" s="27"/>
       <c r="E96" s="27"/>
@@ -7375,7 +7378,7 @@
       <c r="I96" s="27"/>
       <c r="J96" s="27"/>
       <c r="K96" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L96" s="22"/>
       <c r="M96" s="27"/>
@@ -7413,10 +7416,10 @@
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="40" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C97" s="22" t="s">
         <v>36</v>
@@ -7516,7 +7519,7 @@
         <v>53</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C99" s="41"/>
       <c r="D99" s="27"/>
@@ -7612,7 +7615,7 @@
         <v>34</v>
       </c>
       <c r="B101" s="46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="47" t="s">
         <v>36</v>
@@ -7626,7 +7629,7 @@
       <c r="J101" s="48"/>
       <c r="K101" s="48"/>
       <c r="L101" s="47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="M101" s="48"/>
       <c r="N101" s="47"/>
@@ -7668,10 +7671,10 @@
         <v>131</v>
       </c>
       <c r="B102" s="46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C102" s="47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D102" s="48"/>
       <c r="E102" s="48"/>
@@ -7720,10 +7723,10 @@
         <v>131</v>
       </c>
       <c r="B103" s="46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C103" s="47" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D103" s="48"/>
       <c r="E103" s="48"/>
@@ -7734,7 +7737,7 @@
       <c r="J103" s="48"/>
       <c r="K103" s="48"/>
       <c r="L103" s="47" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M103" s="48"/>
       <c r="N103" s="48"/>
@@ -7774,10 +7777,10 @@
         <v>131</v>
       </c>
       <c r="B104" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C104" s="51" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D104" s="48"/>
       <c r="E104" s="48"/>
@@ -7826,10 +7829,10 @@
         <v>131</v>
       </c>
       <c r="B105" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C105" s="34" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D105" s="48"/>
       <c r="E105" s="48"/>
@@ -7840,7 +7843,7 @@
       <c r="J105" s="48"/>
       <c r="K105" s="48"/>
       <c r="L105" s="47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M105" s="48"/>
       <c r="N105" s="48"/>
@@ -7880,10 +7883,10 @@
         <v>131</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D106" s="27"/>
       <c r="E106" s="27"/>
@@ -7894,7 +7897,7 @@
       <c r="J106" s="22"/>
       <c r="K106" s="22"/>
       <c r="L106" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M106" s="22"/>
       <c r="N106" s="27"/>
@@ -7934,10 +7937,10 @@
         <v>131</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D107" s="27"/>
       <c r="E107" s="27"/>
@@ -7948,7 +7951,7 @@
       <c r="J107" s="22"/>
       <c r="K107" s="22"/>
       <c r="L107" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M107" s="22"/>
       <c r="N107" s="27"/>
@@ -7988,10 +7991,10 @@
         <v>131</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D108" s="27"/>
       <c r="E108" s="27"/>
@@ -8002,7 +8005,7 @@
       <c r="J108" s="22"/>
       <c r="K108" s="22"/>
       <c r="L108" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M108" s="22"/>
       <c r="N108" s="27"/>
@@ -8042,10 +8045,10 @@
         <v>131</v>
       </c>
       <c r="B109" s="20" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D109" s="27"/>
       <c r="E109" s="27"/>
@@ -8056,7 +8059,7 @@
       <c r="J109" s="22"/>
       <c r="K109" s="22"/>
       <c r="L109" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M109" s="22"/>
       <c r="N109" s="27"/>
@@ -8096,10 +8099,10 @@
         <v>131</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D110" s="27"/>
       <c r="E110" s="27"/>
@@ -8110,7 +8113,7 @@
       <c r="J110" s="22"/>
       <c r="K110" s="22"/>
       <c r="L110" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M110" s="22"/>
       <c r="N110" s="27"/>
@@ -8150,10 +8153,10 @@
         <v>131</v>
       </c>
       <c r="B111" s="52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C111" s="34" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D111" s="48"/>
       <c r="E111" s="48"/>
@@ -8163,10 +8166,10 @@
       <c r="I111" s="48"/>
       <c r="J111" s="48"/>
       <c r="K111" s="34" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L111" s="47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M111" s="48"/>
       <c r="N111" s="48"/>
@@ -8206,10 +8209,10 @@
         <v>131</v>
       </c>
       <c r="B112" s="52" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C112" s="53" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D112" s="54"/>
       <c r="E112" s="54"/>
@@ -8219,10 +8222,10 @@
       <c r="I112" s="54"/>
       <c r="J112" s="50"/>
       <c r="K112" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L112" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M112" s="50"/>
       <c r="N112" s="50"/>
@@ -8262,10 +8265,10 @@
         <v>131</v>
       </c>
       <c r="B113" s="52" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C113" s="53" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D113" s="27"/>
       <c r="E113" s="27"/>
@@ -8275,10 +8278,10 @@
       <c r="I113" s="27"/>
       <c r="J113" s="22"/>
       <c r="K113" s="34" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L113" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M113" s="22"/>
       <c r="N113" s="27"/>
@@ -8318,10 +8321,10 @@
         <v>131</v>
       </c>
       <c r="B114" s="52" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C114" s="53" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D114" s="27"/>
       <c r="E114" s="27"/>
@@ -8331,10 +8334,10 @@
       <c r="I114" s="27"/>
       <c r="J114" s="22"/>
       <c r="K114" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L114" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M114" s="22"/>
       <c r="N114" s="27"/>
@@ -8374,10 +8377,10 @@
         <v>131</v>
       </c>
       <c r="B115" s="52" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C115" s="53" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D115" s="27"/>
       <c r="E115" s="27"/>
@@ -8387,10 +8390,10 @@
       <c r="I115" s="27"/>
       <c r="J115" s="22"/>
       <c r="K115" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L115" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M115" s="22"/>
       <c r="N115" s="27"/>
@@ -8430,10 +8433,10 @@
         <v>131</v>
       </c>
       <c r="B116" s="52" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C116" s="53" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D116" s="27"/>
       <c r="E116" s="27"/>
@@ -8443,10 +8446,10 @@
       <c r="I116" s="27"/>
       <c r="J116" s="22"/>
       <c r="K116" s="34" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L116" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M116" s="22"/>
       <c r="N116" s="27"/>
@@ -8486,10 +8489,10 @@
         <v>131</v>
       </c>
       <c r="B117" s="52" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D117" s="27"/>
       <c r="E117" s="27"/>
@@ -8499,10 +8502,10 @@
       <c r="I117" s="27"/>
       <c r="J117" s="22"/>
       <c r="K117" s="34" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L117" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M117" s="22"/>
       <c r="N117" s="27"/>
@@ -8542,10 +8545,10 @@
         <v>131</v>
       </c>
       <c r="B118" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D118" s="27"/>
       <c r="E118" s="27"/>
@@ -8555,10 +8558,10 @@
       <c r="I118" s="27"/>
       <c r="J118" s="27"/>
       <c r="K118" s="56" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L118" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M118" s="27"/>
       <c r="N118" s="28"/>
@@ -8598,10 +8601,10 @@
         <v>131</v>
       </c>
       <c r="B119" s="52" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C119" s="34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D119" s="48"/>
       <c r="E119" s="48"/>
@@ -8611,10 +8614,10 @@
       <c r="I119" s="48"/>
       <c r="J119" s="48"/>
       <c r="K119" s="34" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L119" s="47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M119" s="48"/>
       <c r="N119" s="48"/>
@@ -8654,10 +8657,10 @@
         <v>131</v>
       </c>
       <c r="B120" s="52" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C120" s="57" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D120" s="54"/>
       <c r="E120" s="54"/>
@@ -8667,10 +8670,10 @@
       <c r="I120" s="54"/>
       <c r="J120" s="50"/>
       <c r="K120" s="34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L120" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M120" s="50"/>
       <c r="N120" s="50"/>
@@ -8710,10 +8713,10 @@
         <v>131</v>
       </c>
       <c r="B121" s="52" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C121" s="57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D121" s="54"/>
       <c r="E121" s="54"/>
@@ -8723,10 +8726,10 @@
       <c r="I121" s="54"/>
       <c r="J121" s="50"/>
       <c r="K121" s="34" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L121" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M121" s="50"/>
       <c r="N121" s="50"/>
@@ -8766,10 +8769,10 @@
         <v>131</v>
       </c>
       <c r="B122" s="52" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C122" s="57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D122" s="54"/>
       <c r="E122" s="54"/>
@@ -8779,10 +8782,10 @@
       <c r="I122" s="54"/>
       <c r="J122" s="50"/>
       <c r="K122" s="34" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L122" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M122" s="50"/>
       <c r="N122" s="50"/>
@@ -8822,10 +8825,10 @@
         <v>131</v>
       </c>
       <c r="B123" s="52" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C123" s="57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D123" s="54"/>
       <c r="E123" s="54"/>
@@ -8835,10 +8838,10 @@
       <c r="I123" s="54"/>
       <c r="J123" s="50"/>
       <c r="K123" s="34" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L123" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M123" s="50"/>
       <c r="N123" s="50"/>
@@ -8878,10 +8881,10 @@
         <v>131</v>
       </c>
       <c r="B124" s="52" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C124" s="57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D124" s="54"/>
       <c r="E124" s="54"/>
@@ -8891,10 +8894,10 @@
       <c r="I124" s="54"/>
       <c r="J124" s="50"/>
       <c r="K124" s="34" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L124" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M124" s="50"/>
       <c r="N124" s="50"/>
@@ -8934,10 +8937,10 @@
         <v>131</v>
       </c>
       <c r="B125" s="52" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C125" s="57" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D125" s="54"/>
       <c r="E125" s="54"/>
@@ -8947,10 +8950,10 @@
       <c r="I125" s="54"/>
       <c r="J125" s="50"/>
       <c r="K125" s="34" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L125" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M125" s="50"/>
       <c r="N125" s="50"/>
@@ -8990,10 +8993,10 @@
         <v>131</v>
       </c>
       <c r="B126" s="52" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C126" s="57" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D126" s="54"/>
       <c r="E126" s="54"/>
@@ -9003,10 +9006,10 @@
       <c r="I126" s="54"/>
       <c r="J126" s="50"/>
       <c r="K126" s="34" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L126" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M126" s="50"/>
       <c r="N126" s="50"/>
@@ -9046,10 +9049,10 @@
         <v>131</v>
       </c>
       <c r="B127" s="52" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C127" s="57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D127" s="54"/>
       <c r="E127" s="54"/>
@@ -9059,10 +9062,10 @@
       <c r="I127" s="54"/>
       <c r="J127" s="50"/>
       <c r="K127" s="34" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L127" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M127" s="50"/>
       <c r="N127" s="50"/>
@@ -9102,10 +9105,10 @@
         <v>131</v>
       </c>
       <c r="B128" s="52" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C128" s="57" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D128" s="54"/>
       <c r="E128" s="54"/>
@@ -9115,10 +9118,10 @@
       <c r="I128" s="54"/>
       <c r="J128" s="50"/>
       <c r="K128" s="34" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L128" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M128" s="50"/>
       <c r="N128" s="50"/>
@@ -9158,10 +9161,10 @@
         <v>131</v>
       </c>
       <c r="B129" s="52" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C129" s="57" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D129" s="54"/>
       <c r="E129" s="54"/>
@@ -9171,10 +9174,10 @@
       <c r="I129" s="54"/>
       <c r="J129" s="50"/>
       <c r="K129" s="34" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L129" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M129" s="50"/>
       <c r="N129" s="50"/>
@@ -9214,10 +9217,10 @@
         <v>131</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D130" s="27"/>
       <c r="E130" s="27"/>
@@ -9227,10 +9230,10 @@
       <c r="I130" s="27"/>
       <c r="J130" s="27"/>
       <c r="K130" s="56" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L130" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M130" s="27"/>
       <c r="N130" s="28"/>
@@ -9270,10 +9273,10 @@
         <v>131</v>
       </c>
       <c r="B131" s="52" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C131" s="57" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D131" s="54"/>
       <c r="E131" s="54"/>
@@ -9283,10 +9286,10 @@
       <c r="I131" s="54"/>
       <c r="J131" s="50"/>
       <c r="K131" s="34" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="L131" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M131" s="50"/>
       <c r="N131" s="50"/>
@@ -9326,10 +9329,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="52" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C132" s="57" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D132" s="54"/>
       <c r="E132" s="54"/>
@@ -9339,10 +9342,10 @@
       <c r="I132" s="54"/>
       <c r="J132" s="50"/>
       <c r="K132" s="34" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L132" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M132" s="50"/>
       <c r="N132" s="50"/>
@@ -9382,10 +9385,10 @@
         <v>131</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D133" s="27"/>
       <c r="E133" s="27"/>
@@ -9395,10 +9398,10 @@
       <c r="I133" s="27"/>
       <c r="J133" s="27"/>
       <c r="K133" s="56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L133" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M133" s="27"/>
       <c r="N133" s="28"/>
@@ -9438,10 +9441,10 @@
         <v>131</v>
       </c>
       <c r="B134" s="52" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C134" s="34" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D134" s="48"/>
       <c r="E134" s="48"/>
@@ -9452,7 +9455,7 @@
       <c r="J134" s="48"/>
       <c r="K134" s="34"/>
       <c r="L134" s="34" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M134" s="48"/>
       <c r="N134" s="48"/>
@@ -9492,10 +9495,10 @@
         <v>131</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D135" s="27"/>
       <c r="E135" s="27"/>
@@ -9506,7 +9509,7 @@
       <c r="J135" s="27"/>
       <c r="K135" s="58"/>
       <c r="L135" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M135" s="27"/>
       <c r="N135" s="28"/>
@@ -9594,7 +9597,7 @@
         <v>34</v>
       </c>
       <c r="B137" s="59" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C137" s="60" t="s">
         <v>36</v>
@@ -9650,7 +9653,7 @@
         <v>34</v>
       </c>
       <c r="B138" s="62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C138" s="60" t="s">
         <v>36</v>
@@ -9702,7 +9705,7 @@
         <v>71</v>
       </c>
       <c r="B139" s="59" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C139" s="60" t="s">
         <v>36</v>
@@ -9725,7 +9728,7 @@
       <c r="S139" s="60"/>
       <c r="T139" s="60"/>
       <c r="U139" s="60" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="V139" s="60"/>
       <c r="W139" s="60"/>
@@ -9740,7 +9743,7 @@
       <c r="AF139" s="60"/>
       <c r="AG139" s="60"/>
       <c r="AH139" s="60" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AI139" s="60"/>
       <c r="AJ139" s="60"/>
@@ -9758,7 +9761,7 @@
         <v>71</v>
       </c>
       <c r="B140" s="59" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C140" s="60" t="s">
         <v>36</v>
@@ -9781,7 +9784,7 @@
       <c r="S140" s="60"/>
       <c r="T140" s="60"/>
       <c r="U140" s="60" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="V140" s="60"/>
       <c r="W140" s="60"/>
@@ -9814,7 +9817,7 @@
         <v>71</v>
       </c>
       <c r="B141" s="59" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C141" s="60" t="s">
         <v>36</v>
@@ -9837,7 +9840,7 @@
       <c r="S141" s="60"/>
       <c r="T141" s="60"/>
       <c r="U141" s="60" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="V141" s="60"/>
       <c r="W141" s="60"/>
@@ -9852,7 +9855,7 @@
       <c r="AF141" s="60"/>
       <c r="AG141" s="60"/>
       <c r="AH141" s="60" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AI141" s="60"/>
       <c r="AJ141" s="60"/>
@@ -9870,7 +9873,7 @@
         <v>71</v>
       </c>
       <c r="B142" s="59" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C142" s="60" t="s">
         <v>36</v>
@@ -9893,7 +9896,7 @@
       <c r="S142" s="60"/>
       <c r="T142" s="60"/>
       <c r="U142" s="60" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="V142" s="60"/>
       <c r="W142" s="60"/>
@@ -9926,7 +9929,7 @@
         <v>71</v>
       </c>
       <c r="B143" s="59" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C143" s="60" t="s">
         <v>36</v>
@@ -9949,7 +9952,7 @@
       <c r="S143" s="60"/>
       <c r="T143" s="60"/>
       <c r="U143" s="60" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="V143" s="60"/>
       <c r="W143" s="60"/>
@@ -9964,7 +9967,7 @@
       <c r="AF143" s="60"/>
       <c r="AG143" s="60"/>
       <c r="AH143" s="60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AI143" s="60"/>
       <c r="AJ143" s="60"/>
@@ -9982,7 +9985,7 @@
         <v>53</v>
       </c>
       <c r="B144" s="62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C144" s="60"/>
       <c r="D144" s="60"/>
@@ -10032,7 +10035,7 @@
         <v>53</v>
       </c>
       <c r="B145" s="62" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C145" s="60"/>
       <c r="D145" s="60"/>
@@ -41344,7 +41347,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="63" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B1" s="63" t="s">
         <v>1</v>
@@ -41376,13 +41379,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="65" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B2" s="65" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D2" s="65"/>
       <c r="E2" s="65"/>
@@ -41406,13 +41409,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="65" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D3" s="65"/>
       <c r="E3" s="65"/>
@@ -41466,7 +41469,7 @@
         <v>111</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
@@ -41493,10 +41496,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C6" s="69" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D6" s="65"/>
       <c r="E6" s="65"/>
@@ -41547,10 +41550,10 @@
         <v>93</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C8" s="68" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
@@ -41579,7 +41582,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -41605,10 +41608,10 @@
         <v>93</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C10" s="68" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -41634,10 +41637,10 @@
         <v>93</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C11" s="68" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -41686,10 +41689,10 @@
         <v>96</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D13" s="71"/>
       <c r="E13" s="72"/>
@@ -41720,10 +41723,10 @@
         <v>96</v>
       </c>
       <c r="B14" s="71" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C14" s="71" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="72"/>
@@ -41754,10 +41757,10 @@
         <v>96</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D15" s="71"/>
       <c r="E15" s="72"/>
@@ -41788,10 +41791,10 @@
         <v>96</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D16" s="71"/>
       <c r="E16" s="72"/>
@@ -41822,10 +41825,10 @@
         <v>96</v>
       </c>
       <c r="B17" s="71" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D17" s="71"/>
       <c r="E17" s="72"/>
@@ -41856,10 +41859,10 @@
         <v>96</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D18" s="71"/>
       <c r="E18" s="72"/>
@@ -41890,10 +41893,10 @@
         <v>96</v>
       </c>
       <c r="B19" s="71" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D19" s="71"/>
       <c r="E19" s="72"/>
@@ -41924,10 +41927,10 @@
         <v>96</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D20" s="71"/>
       <c r="E20" s="72"/>
@@ -41958,10 +41961,10 @@
         <v>96</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C21" s="71" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D21" s="71"/>
       <c r="E21" s="72"/>
@@ -41992,10 +41995,10 @@
         <v>96</v>
       </c>
       <c r="B22" s="71" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D22" s="71"/>
       <c r="E22" s="72"/>
@@ -42026,10 +42029,10 @@
         <v>96</v>
       </c>
       <c r="B23" s="71" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C23" s="71" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D23" s="71"/>
       <c r="E23" s="72"/>
@@ -42060,10 +42063,10 @@
         <v>96</v>
       </c>
       <c r="B24" s="71" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C24" s="71" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D24" s="71"/>
       <c r="E24" s="72"/>
@@ -42094,10 +42097,10 @@
         <v>96</v>
       </c>
       <c r="B25" s="71" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C25" s="71" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D25" s="71"/>
       <c r="E25" s="72"/>
@@ -42128,10 +42131,10 @@
         <v>96</v>
       </c>
       <c r="B26" s="71" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C26" s="71" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D26" s="71"/>
       <c r="E26" s="72"/>
@@ -42162,10 +42165,10 @@
         <v>96</v>
       </c>
       <c r="B27" s="71" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C27" s="71" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D27" s="71"/>
       <c r="E27" s="72"/>
@@ -42196,10 +42199,10 @@
         <v>96</v>
       </c>
       <c r="B28" s="71" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D28" s="71"/>
       <c r="E28" s="72"/>
@@ -42230,10 +42233,10 @@
         <v>96</v>
       </c>
       <c r="B29" s="71" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="72"/>
@@ -42264,10 +42267,10 @@
         <v>96</v>
       </c>
       <c r="B30" s="71" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C30" s="71" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D30" s="71"/>
       <c r="E30" s="72"/>
@@ -42298,10 +42301,10 @@
         <v>96</v>
       </c>
       <c r="B31" s="71" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C31" s="71" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D31" s="71"/>
       <c r="E31" s="72"/>
@@ -42332,10 +42335,10 @@
         <v>96</v>
       </c>
       <c r="B32" s="71" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C32" s="71" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D32" s="71"/>
       <c r="E32" s="72"/>
@@ -42366,10 +42369,10 @@
         <v>96</v>
       </c>
       <c r="B33" s="71" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C33" s="71" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D33" s="71"/>
       <c r="E33" s="72"/>
@@ -42400,10 +42403,10 @@
         <v>96</v>
       </c>
       <c r="B34" s="71" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D34" s="71"/>
       <c r="E34" s="72"/>
@@ -42434,10 +42437,10 @@
         <v>96</v>
       </c>
       <c r="B35" s="71" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D35" s="71"/>
       <c r="E35" s="72"/>
@@ -42468,10 +42471,10 @@
         <v>96</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D36" s="71"/>
       <c r="E36" s="72"/>
@@ -42502,10 +42505,10 @@
         <v>96</v>
       </c>
       <c r="B37" s="71" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D37" s="71"/>
       <c r="E37" s="72"/>
@@ -42536,10 +42539,10 @@
         <v>96</v>
       </c>
       <c r="B38" s="71" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="72"/>
@@ -42570,10 +42573,10 @@
         <v>96</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C39" s="71" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D39" s="71"/>
       <c r="E39" s="72"/>
@@ -42604,10 +42607,10 @@
         <v>96</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D40" s="71"/>
       <c r="E40" s="72"/>
@@ -42638,10 +42641,10 @@
         <v>96</v>
       </c>
       <c r="B41" s="71" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D41" s="71"/>
       <c r="E41" s="72"/>
@@ -42672,10 +42675,10 @@
         <v>96</v>
       </c>
       <c r="B42" s="71" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D42" s="71"/>
       <c r="E42" s="72"/>
@@ -42706,10 +42709,10 @@
         <v>96</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D43" s="71"/>
       <c r="E43" s="72"/>
@@ -42740,10 +42743,10 @@
         <v>96</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D44" s="71"/>
       <c r="E44" s="72"/>
@@ -42774,10 +42777,10 @@
         <v>96</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D45" s="71"/>
       <c r="E45" s="72"/>
@@ -42808,10 +42811,10 @@
         <v>96</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D46" s="71"/>
       <c r="E46" s="72"/>
@@ -42842,10 +42845,10 @@
         <v>96</v>
       </c>
       <c r="B47" s="71" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D47" s="71"/>
       <c r="E47" s="72"/>
@@ -42876,10 +42879,10 @@
         <v>96</v>
       </c>
       <c r="B48" s="71" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D48" s="71"/>
       <c r="E48" s="72"/>
@@ -42910,10 +42913,10 @@
         <v>96</v>
       </c>
       <c r="B49" s="71" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C49" s="71" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D49" s="71"/>
       <c r="E49" s="72"/>
@@ -42944,10 +42947,10 @@
         <v>96</v>
       </c>
       <c r="B50" s="71" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C50" s="71" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D50" s="71"/>
       <c r="E50" s="72"/>
@@ -42978,10 +42981,10 @@
         <v>96</v>
       </c>
       <c r="B51" s="71" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C51" s="71" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D51" s="71"/>
       <c r="E51" s="72"/>
@@ -43012,10 +43015,10 @@
         <v>96</v>
       </c>
       <c r="B52" s="71" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C52" s="71" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D52" s="71"/>
       <c r="E52" s="72"/>
@@ -43046,10 +43049,10 @@
         <v>96</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C53" s="71" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D53" s="71"/>
       <c r="E53" s="72"/>
@@ -43080,10 +43083,10 @@
         <v>96</v>
       </c>
       <c r="B54" s="71" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C54" s="71" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D54" s="71"/>
       <c r="E54" s="72"/>
@@ -43114,10 +43117,10 @@
         <v>96</v>
       </c>
       <c r="B55" s="71" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C55" s="71" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D55" s="71"/>
       <c r="E55" s="72"/>
@@ -43148,10 +43151,10 @@
         <v>96</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C56" s="71" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D56" s="71"/>
       <c r="E56" s="72"/>
@@ -43182,10 +43185,10 @@
         <v>96</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C57" s="71" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D57" s="71"/>
       <c r="E57" s="72"/>
@@ -43216,10 +43219,10 @@
         <v>96</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C58" s="71" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D58" s="71"/>
       <c r="E58" s="72"/>
@@ -43250,10 +43253,10 @@
         <v>96</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C59" s="71" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D59" s="71"/>
       <c r="E59" s="72"/>
@@ -43306,10 +43309,10 @@
         <v>116</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C61" s="57" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D61" s="39"/>
       <c r="E61" s="39"/>
@@ -43335,10 +43338,10 @@
         <v>116</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C62" s="57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D62" s="39"/>
       <c r="E62" s="39"/>
@@ -43364,10 +43367,10 @@
         <v>116</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C63" s="57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D63" s="39"/>
       <c r="E63" s="39"/>
@@ -43393,10 +43396,10 @@
         <v>116</v>
       </c>
       <c r="B64" s="57" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C64" s="57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D64" s="39"/>
       <c r="E64" s="39"/>
@@ -43422,10 +43425,10 @@
         <v>116</v>
       </c>
       <c r="B65" s="57" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C65" s="57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D65" s="39"/>
       <c r="E65" s="39"/>
@@ -43451,10 +43454,10 @@
         <v>116</v>
       </c>
       <c r="B66" s="57" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D66" s="39"/>
       <c r="E66" s="39"/>
@@ -43480,10 +43483,10 @@
         <v>116</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C67" s="57" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D67" s="39"/>
       <c r="E67" s="39"/>
@@ -43509,10 +43512,10 @@
         <v>116</v>
       </c>
       <c r="B68" s="57" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C68" s="57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D68" s="39"/>
       <c r="E68" s="39"/>
@@ -43538,10 +43541,10 @@
         <v>116</v>
       </c>
       <c r="B69" s="57" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C69" s="57" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D69" s="39"/>
       <c r="E69" s="39"/>
@@ -43567,10 +43570,10 @@
         <v>116</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C70" s="57" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D70" s="39"/>
       <c r="E70" s="39"/>
@@ -43619,10 +43622,10 @@
         <v>106</v>
       </c>
       <c r="B72" s="53" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C72" s="53" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D72" s="39"/>
       <c r="E72" s="39"/>
@@ -43648,10 +43651,10 @@
         <v>106</v>
       </c>
       <c r="B73" s="53" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C73" s="53" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D73" s="39"/>
       <c r="E73" s="39"/>
@@ -43677,10 +43680,10 @@
         <v>106</v>
       </c>
       <c r="B74" s="53" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C74" s="53" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D74" s="39"/>
       <c r="E74" s="39"/>
@@ -43706,10 +43709,10 @@
         <v>106</v>
       </c>
       <c r="B75" s="53" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C75" s="53" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D75" s="39"/>
       <c r="E75" s="39"/>
@@ -43735,10 +43738,10 @@
         <v>106</v>
       </c>
       <c r="B76" s="53" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C76" s="53" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D76" s="39"/>
       <c r="E76" s="39"/>
@@ -43764,10 +43767,10 @@
         <v>106</v>
       </c>
       <c r="B77" s="53" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C77" s="53" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D77" s="39"/>
       <c r="E77" s="39"/>
@@ -43813,13 +43816,13 @@
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B79" s="76" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C79" s="76" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D79" s="39"/>
       <c r="E79" s="39"/>
@@ -43842,13 +43845,13 @@
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B80" s="76" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C80" s="76" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D80" s="39"/>
       <c r="E80" s="39"/>
@@ -43871,13 +43874,13 @@
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B81" s="76" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C81" s="76" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D81" s="39"/>
       <c r="E81" s="39"/>
@@ -43900,13 +43903,13 @@
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B82" s="76" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C82" s="76" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D82" s="39"/>
       <c r="E82" s="39"/>
@@ -43929,13 +43932,13 @@
     </row>
     <row r="83" ht="12.75" customHeight="1">
       <c r="A83" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B83" s="76" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C83" s="76" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D83" s="39"/>
       <c r="E83" s="39"/>
@@ -43958,13 +43961,13 @@
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B84" s="76" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C84" s="76" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D84" s="39"/>
       <c r="E84" s="39"/>
@@ -51305,25 +51308,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="77" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B1" s="77" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C1" s="77" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F1" s="77" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H1" s="77"/>
       <c r="I1" s="77"/>
@@ -51347,24 +51350,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="79" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C2" s="80">
         <f>NOW()</f>
-        <v>45094.20004</v>
+        <v>45121.07195</v>
       </c>
       <c r="D2" s="81" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E2" s="81" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F2" s="66"/>
       <c r="G2" s="82" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
@@ -52412,7 +52415,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="77" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B1" s="77" t="s">
         <v>1</v>
@@ -52455,13 +52458,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="67" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D2" s="67"/>
       <c r="E2" s="67"/>
@@ -52486,13 +52489,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="67" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C3" s="67" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D3" s="67"/>
       <c r="E3" s="67"/>
@@ -52542,13 +52545,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="67" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D5" s="67"/>
       <c r="E5" s="67"/>
@@ -52573,13 +52576,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="67" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D6" s="67"/>
       <c r="E6" s="67"/>
@@ -52604,13 +52607,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="67" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D7" s="67"/>
       <c r="E7" s="67"/>
@@ -52635,13 +52638,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="67" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B8" s="67" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D8" s="67"/>
       <c r="E8" s="67"/>
@@ -52666,13 +52669,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="67" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B9" s="67" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D9" s="67"/>
       <c r="E9" s="67"/>
@@ -52722,13 +52725,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B11" s="67" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D11" s="67"/>
       <c r="E11" s="67"/>
@@ -52753,13 +52756,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D12" s="67"/>
       <c r="E12" s="67"/>
@@ -52784,13 +52787,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D13" s="67"/>
       <c r="E13" s="67"/>
@@ -52815,13 +52818,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B14" s="67" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D14" s="67"/>
       <c r="E14" s="67"/>
@@ -52846,13 +52849,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B15" s="67" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D15" s="67"/>
       <c r="E15" s="67"/>
@@ -52877,13 +52880,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="67" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B16" s="67" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D16" s="67"/>
       <c r="E16" s="67"/>
@@ -52933,13 +52936,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B18" s="67" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D18" s="67"/>
       <c r="E18" s="67"/>
@@ -52964,13 +52967,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D19" s="67"/>
       <c r="E19" s="67"/>
@@ -52995,13 +52998,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D20" s="67"/>
       <c r="E20" s="67"/>
@@ -53026,13 +53029,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B21" s="67" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C21" s="67" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D21" s="67"/>
       <c r="E21" s="67"/>
@@ -53057,13 +53060,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="67" t="s">
+        <v>431</v>
+      </c>
+      <c r="B22" s="67" t="s">
+        <v>429</v>
+      </c>
+      <c r="C22" s="67" t="s">
         <v>430</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>428</v>
-      </c>
-      <c r="C22" s="67" t="s">
-        <v>429</v>
       </c>
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
@@ -53088,13 +53091,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D23" s="67"/>
       <c r="E23" s="67"/>
@@ -53144,13 +53147,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B25" s="67" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D25" s="67"/>
       <c r="E25" s="67"/>
@@ -53175,13 +53178,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B26" s="67" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C26" s="67" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D26" s="67"/>
       <c r="E26" s="67"/>
@@ -53206,13 +53209,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B27" s="67" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D27" s="67"/>
       <c r="E27" s="67"/>
@@ -53237,13 +53240,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="67"/>
@@ -53268,13 +53271,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B29" s="67" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C29" s="67" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D29" s="67"/>
       <c r="E29" s="67"/>
@@ -53324,13 +53327,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="67" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B31" s="67" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C31" s="67" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D31" s="67"/>
       <c r="E31" s="67"/>
@@ -53355,13 +53358,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="67" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B32" s="67" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D32" s="67"/>
       <c r="E32" s="67"/>
@@ -53411,121 +53414,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B34" s="90" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" s="90" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B35" s="90" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" s="90" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B36" s="90" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" s="90" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B37" s="90" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" s="90" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B38" s="90" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" s="90" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B39" s="90" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" s="90" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B40" s="90" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" s="90" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B41" s="90" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" s="90" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B42" s="90" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" s="90" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="90" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B43" s="90" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C43" s="90" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -53536,26 +53539,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="90" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B45" s="90" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" s="90" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="90" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B46" s="90" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" s="90" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -53566,13 +53569,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="81" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B48" s="81" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C48" s="81" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="81"/>
@@ -53597,13 +53600,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="81" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B49" s="81" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C49" s="81" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D49" s="81"/>
       <c r="E49" s="81"/>
@@ -53629,226 +53632,226 @@
     <row r="50" ht="12.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B51" s="90" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C51" s="90" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B52" s="90" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C52" s="90" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B53" s="90" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C53" s="90" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B54" s="90" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C54" s="90" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B55" s="90" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C55" s="90" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="90" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B56" s="90" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C56" s="90" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="81" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B58" s="81" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C58" s="81" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="81" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B59" s="81" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C59" s="81" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="81" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B60" s="81" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C60" s="81" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="81" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B61" s="81" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C61" s="81" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62" ht="12.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B63" s="66" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C63" s="81" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B64" s="66" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C64" s="81" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B65" s="66" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C65" s="81" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B66" s="66" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C66" s="81" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B67" s="66" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C67" s="81" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="90" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B69" s="90" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C69" s="90" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="90" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B70" s="90" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C70" s="90" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" ht="12.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="90" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B72" s="90" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C72" s="91" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="90" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B73" s="90" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C73" s="90" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="90" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B74" s="90" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C74" s="90" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
pass data to padr report:
</commit_message>
<xml_diff>
--- a/cht_app/forms/app/padr.xlsx
+++ b/cht_app/forms/app/padr.xlsx
@@ -687,7 +687,7 @@
     <t>r_absent</t>
   </si>
   <si>
-    <t>&lt;b&gt;Revisit ${patient_display_name} in the next 5 days&lt;/b&gt;</t>
+    <t>&lt;b&gt;Revisit ${patient_display_name} within 5 days&lt;/b&gt;</t>
   </si>
   <si>
     <t>selected(${available},'No')</t>
@@ -49230,7 +49230,7 @@
       </c>
       <c r="C2" s="102">
         <f>NOW()</f>
-        <v>45170.20223</v>
+        <v>45175.1402</v>
       </c>
       <c r="D2" s="103" t="s">
         <v>345</v>

</xml_diff>